<commit_message>
Uploaded 03-九月-2019 13:50:30 {/src/main/resources/com/redhat/prudential_poc/UW_Rule.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/UW_Rule.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/UW_Rule.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83422C78-6DB0-9B4A-8E18-5AED52E944FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F150951-285E-C249-BDA3-F80A9156C04F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37520" yWindow="480" windowWidth="37540" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
   <sheets>
-    <sheet name="黑名單" sheetId="3" r:id="rId1"/>
-    <sheet name="免體檢" sheetId="1" r:id="rId2"/>
-    <sheet name="既有保戶" sheetId="2" r:id="rId3"/>
+    <sheet name="blacklist" sheetId="3" r:id="rId1"/>
+    <sheet name="nohealthcheck" sheetId="1" r:id="rId2"/>
+    <sheet name="policy" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>RuleSet</t>
   </si>
@@ -288,6 +288,10 @@
   </si>
   <si>
     <t>nohtc-rule4</t>
+  </si>
+  <si>
+    <t>nohealthcheck</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -890,7 +894,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1032,7 +1036,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1189,7 +1193,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1272,7 +1276,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>